<commit_message>
Archivo datos modificado y los graficos
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costarica95\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/adbab69e72667606/Documents/Universidad/IS-2023/Herramientas para ciencias de datos II/Proyecto/Proyecto_Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0CE968-D42E-46D7-9CE2-2D712D8CEE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{8A0CE968-D42E-46D7-9CE2-2D712D8CEE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF7A6532-BBC4-428A-B70C-E2A32B178851}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -37,39 +37,6 @@
     <t>Enero</t>
   </si>
   <si>
-    <t> Febrero</t>
-  </si>
-  <si>
-    <t> Marzo</t>
-  </si>
-  <si>
-    <t> Abril</t>
-  </si>
-  <si>
-    <t> Mayo</t>
-  </si>
-  <si>
-    <t> Junio</t>
-  </si>
-  <si>
-    <t> Julio</t>
-  </si>
-  <si>
-    <t> Agosto</t>
-  </si>
-  <si>
-    <t> Septiembre</t>
-  </si>
-  <si>
-    <t> Octubre</t>
-  </si>
-  <si>
-    <t> Noviembre</t>
-  </si>
-  <si>
-    <t> Diciembre</t>
-  </si>
-  <si>
     <t>IPC_Nivel</t>
   </si>
   <si>
@@ -80,6 +47,39 @@
   </si>
   <si>
     <t>IMAE_ULT_12M</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Mayo</t>
   </si>
 </sst>
 </file>
@@ -472,14 +472,14 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -498,16 +498,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>2018</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>2018</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>2018</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>2018</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>2018</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>2018</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>2018</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>2018</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>2018</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>2018</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>2018</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1">
         <v>2019</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1">
         <v>2019</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1">
         <v>2019</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>2019</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1">
         <v>2019</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1">
         <v>2019</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1">
         <v>2019</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1">
         <v>2019</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
         <v>2019</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1">
         <v>2019</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1">
         <v>2019</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B27" s="1">
         <v>2020</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B28" s="1">
         <v>2020</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B29" s="1">
         <v>2020</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B30" s="1">
         <v>2020</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1">
         <v>2020</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B32" s="1">
         <v>2020</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1">
         <v>2020</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1">
         <v>2020</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1">
         <v>2020</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B36" s="1">
         <v>2020</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B37" s="1">
         <v>2020</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B39" s="1">
         <v>2021</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B40" s="1">
         <v>2021</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B41" s="1">
         <v>2021</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B42" s="1">
         <v>2021</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B43" s="1">
         <v>2021</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B44" s="1">
         <v>2021</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B45" s="1">
         <v>2021</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B46" s="1">
         <v>2021</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B47" s="1">
         <v>2021</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B48" s="1">
         <v>2021</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B49" s="1">
         <v>2021</v>
@@ -1802,6 +1802,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>